<commit_message>
Prettify connections.xml for easier editing/diffing
</commit_message>
<xml_diff>
--- a/external-data-blank.xlsx
+++ b/external-data-blank.xlsx
@@ -23,8 +23,8 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <connection id="1" name="External data URL" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr prompt="0" codePage="65001" sourceFile="http://localhost:3000/experiment/10/csv" tab="0" comma="1">
+  <connection background="1" id="1" name="External data URL" refreshedVersion="0" saveData="1" type="6">
+    <textPr codePage="65001" comma="1" prompt="0" sourceFile="http://localhost:3000/experiment/10/csv" tab="0">
       <textFields count="14">
         <textField/>
         <textField/>

</xml_diff>